<commit_message>
donation group then email upload is working
</commit_message>
<xml_diff>
--- a/D:\test excel\Import1.xlsx
+++ b/D:\test excel\Import1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63215979-386E-1D48-9E9F-E3F77A993DA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4670B64-020D-C946-AD47-33D2D977B46C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="2000" windowWidth="24240" windowHeight="12680" xr2:uid="{CD9DBED5-F693-1548-8857-4277C8EC554B}"/>
   </bookViews>
@@ -34,105 +34,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
-  <si>
-    <t>Receipt ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Recurring Total Months</t>
-  </si>
-  <si>
-    <t>Recurrence Number</t>
-  </si>
-  <si>
-    <t>Reference Code</t>
-  </si>
-  <si>
-    <t>Donor First Name</t>
-  </si>
-  <si>
-    <t>Donor Last Name</t>
-  </si>
-  <si>
-    <t>Donor Addr1</t>
-  </si>
-  <si>
-    <t>Donor Addr2</t>
-  </si>
-  <si>
-    <t>Donor City</t>
-  </si>
-  <si>
-    <t>Donor State</t>
-  </si>
-  <si>
-    <t>Donor ZIP</t>
-  </si>
-  <si>
-    <t>Donor Country</t>
-  </si>
-  <si>
-    <t>Donor Email</t>
-  </si>
-  <si>
-    <t>unlimited</t>
-  </si>
-  <si>
-    <t>Margot</t>
-  </si>
-  <si>
-    <t>Sondgeroth</t>
-  </si>
-  <si>
-    <t>2214 N. 22nd St</t>
-  </si>
-  <si>
-    <t>Lafayette</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>wabashriver1@gmail.com</t>
-  </si>
-  <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>Tulowitzki</t>
-  </si>
-  <si>
-    <t>8808 Northcote Ave</t>
-  </si>
-  <si>
-    <t>Munster</t>
-  </si>
-  <si>
-    <t>tuloformunster@gmail.com</t>
-  </si>
-  <si>
-    <t>2017-03-03 16:02:18</t>
-  </si>
-  <si>
-    <t>2017-03-03 16:02:19</t>
-  </si>
-  <si>
-    <t>B1009624999409</t>
-  </si>
-  <si>
-    <t>B1009616763000</t>
-  </si>
-  <si>
     <t>backo4</t>
+  </si>
+  <si>
+    <t>backo5</t>
+  </si>
+  <si>
+    <t>Email Name</t>
+  </si>
+  <si>
+    <t>Recipients</t>
+  </si>
+  <si>
+    <t>Recipient List</t>
+  </si>
+  <si>
+    <t>Excluded List</t>
+  </si>
+  <si>
+    <t>Bounces</t>
+  </si>
+  <si>
+    <t>Unsubscribes</t>
+  </si>
+  <si>
+    <t>Unique Clicks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Opens </t>
+  </si>
+  <si>
+    <t>New Subs</t>
+  </si>
+  <si>
+    <t>Do not exclude segments</t>
+  </si>
+  <si>
+    <t>Send to All Subscribers</t>
+  </si>
+  <si>
+    <t>Refcode</t>
+  </si>
+  <si>
+    <t>Backo5</t>
+  </si>
+  <si>
+    <t>Backo4</t>
   </si>
 </sst>
 </file>
@@ -176,7 +128,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A115F82E-833E-9A49-9BB3-88AC8D72074F}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,136 +454,100 @@
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>3845</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44197</v>
+      </c>
+      <c r="F2">
+        <v>216</v>
+      </c>
+      <c r="G2">
+        <v>115</v>
+      </c>
+      <c r="H2">
+        <v>359</v>
+      </c>
+      <c r="I2">
+        <v>1194</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>3673</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44197</v>
+      </c>
+      <c r="F3">
+        <v>86</v>
+      </c>
+      <c r="G3">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>272</v>
+      </c>
+      <c r="I3">
+        <v>798</v>
+      </c>
+      <c r="J3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2">
-        <v>47904</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3">
-        <v>20.21</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3">
-        <v>46321</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new date format working in donation excel
</commit_message>
<xml_diff>
--- a/D:\test excel\Import1.xlsx
+++ b/D:\test excel\Import1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4670B64-020D-C946-AD47-33D2D977B46C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F06B07-9D37-9640-8983-1B9A5604BEE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="2000" windowWidth="24240" windowHeight="12680" xr2:uid="{CD9DBED5-F693-1548-8857-4277C8EC554B}"/>
   </bookViews>
@@ -34,57 +34,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>backo4</t>
-  </si>
-  <si>
-    <t>backo5</t>
-  </si>
-  <si>
-    <t>Email Name</t>
-  </si>
-  <si>
-    <t>Recipients</t>
-  </si>
-  <si>
-    <t>Recipient List</t>
-  </si>
-  <si>
-    <t>Excluded List</t>
-  </si>
-  <si>
-    <t>Bounces</t>
-  </si>
-  <si>
-    <t>Unsubscribes</t>
-  </si>
-  <si>
-    <t>Unique Clicks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique Opens </t>
-  </si>
-  <si>
-    <t>New Subs</t>
-  </si>
-  <si>
-    <t>Do not exclude segments</t>
-  </si>
-  <si>
-    <t>Send to All Subscribers</t>
-  </si>
-  <si>
-    <t>Refcode</t>
-  </si>
-  <si>
-    <t>Backo5</t>
-  </si>
-  <si>
-    <t>Backo4</t>
+    <t>Receipt ID</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Recurring Total Months</t>
+  </si>
+  <si>
+    <t>Recurrence Number</t>
+  </si>
+  <si>
+    <t>Reference Code</t>
+  </si>
+  <si>
+    <t>Donor First Name</t>
+  </si>
+  <si>
+    <t>Donor Last Name</t>
+  </si>
+  <si>
+    <t>Donor Addr1</t>
+  </si>
+  <si>
+    <t>Donor Addr2</t>
+  </si>
+  <si>
+    <t>Donor City</t>
+  </si>
+  <si>
+    <t>Donor State</t>
+  </si>
+  <si>
+    <t>Donor ZIP</t>
+  </si>
+  <si>
+    <t>Donor Email</t>
+  </si>
+  <si>
+    <t>Donor Phone</t>
+  </si>
+  <si>
+    <t>unlimited</t>
+  </si>
+  <si>
+    <t>backontrack.fr.042821</t>
+  </si>
+  <si>
+    <t>Margot</t>
+  </si>
+  <si>
+    <t>Sondgeroth</t>
+  </si>
+  <si>
+    <t>2214 N. 22nd St</t>
+  </si>
+  <si>
+    <t>Lafayette</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>wabashriver1@gmail.com</t>
+  </si>
+  <si>
+    <t>2020-01-28 11:41:51</t>
+  </si>
+  <si>
+    <t>AB19006167630</t>
+  </si>
+  <si>
+    <t>CAB1906167630</t>
   </si>
 </sst>
 </file>
@@ -128,7 +155,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A115F82E-833E-9A49-9BB3-88AC8D72074F}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,100 +481,133 @@
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44318.360972222225</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
-        <v>14</v>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>47904</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
-        <v>3845</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>44197</v>
-      </c>
-      <c r="F2">
-        <v>216</v>
-      </c>
-      <c r="G2">
-        <v>115</v>
-      </c>
-      <c r="H2">
-        <v>359</v>
-      </c>
-      <c r="I2">
-        <v>1194</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3">
+        <v>47904</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3">
-        <v>3673</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1">
-        <v>44197</v>
-      </c>
-      <c r="F3">
-        <v>86</v>
-      </c>
-      <c r="G3">
-        <v>43</v>
-      </c>
-      <c r="H3">
-        <v>272</v>
-      </c>
-      <c r="I3">
-        <v>798</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>